<commit_message>
Deploying to gh-pages from  @ cf13f20221b18ed935c4bae4b84ee1924e3877c9 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/2.3.2.1.xlsx
+++ b/en/downloads/data-excel/2.3.2.1.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t>(процент)</t>
-  </si>
-  <si>
     <t>Доля произведенной продукции сельскохозяйственными кооперативами в общем объеме произведенной продукции в республике</t>
   </si>
   <si>
@@ -36,29 +33,6 @@
   </si>
   <si>
     <t>2.3.2.1  Доля произведенной продукции сельскохозяйственными кооперативами в общем объеме произведенной продукции в республике</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>доля произведенной продукции</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF2B2B2B"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> растениеводства</t>
-    </r>
   </si>
   <si>
     <r>
@@ -96,9 +70,6 @@
     <t>2.3.2.1 Республикада өндүрүлгөн продукциянын жалпы көлөмүндө айыл чарба кооперативдери өндүргөн продукциянын үлүшү</t>
   </si>
   <si>
-    <t>(пайыз)</t>
-  </si>
-  <si>
     <t>2.3.2.1 Proportion of product produced by agricultural cooperatives to total volume of products produced in the country</t>
   </si>
   <si>
@@ -114,9 +85,6 @@
     <t>share of livestock production</t>
   </si>
   <si>
-    <t>Республикада чыгарылып жаткан продукциянын жалпы келемунде айыл чарба кооперативдери чыгарган продукциянын салыштырма салмагы</t>
-  </si>
-  <si>
     <t>Анын ичинде:</t>
   </si>
   <si>
@@ -126,7 +94,36 @@
     <t>мал чарба продукциясынын улушу</t>
   </si>
   <si>
-    <t>(percent)</t>
+    <t>(пайыз менен)</t>
+  </si>
+  <si>
+    <t>(в процентах)</t>
+  </si>
+  <si>
+    <t>(in percent)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>доля произведенной продукции</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2B2B2B"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> растениеводства</t>
+    </r>
+  </si>
+  <si>
+    <t>Республикада өндүрүлгөн продукциянын жалпы көлөмүндө айыл чарба кооперативдери өндүргөн продукциянын үлүшү</t>
   </si>
 </sst>
 </file>
@@ -136,7 +133,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +250,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -286,18 +298,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -333,32 +341,48 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -8134,617 +8158,623 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="47.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="4"/>
-    <col min="5" max="5" width="8.7109375" style="17"/>
-    <col min="6" max="7" width="8.7109375" style="4"/>
-    <col min="8" max="8" width="8.7109375" style="17"/>
-    <col min="9" max="9" width="8.7109375" style="4"/>
-    <col min="10" max="10" width="8.7109375" style="17"/>
-    <col min="11" max="16384" width="8.7109375" style="4"/>
+    <col min="1" max="3" width="43.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="15" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="3"/>
+    <col min="10" max="10" width="8.7109375" style="15"/>
+    <col min="11" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="18">
+        <v>2019</v>
+      </c>
+      <c r="E4" s="18">
+        <v>2020</v>
+      </c>
+      <c r="F4" s="21">
+        <v>2021</v>
+      </c>
+      <c r="G4" s="18">
+        <v>2022</v>
+      </c>
+      <c r="H4" s="18">
+        <v>2023</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" s="25" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D5" s="30">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="30">
+        <v>1.4</v>
+      </c>
+      <c r="F5" s="30">
+        <v>1.6</v>
+      </c>
+      <c r="G5" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H5" s="31">
+        <v>1.3</v>
+      </c>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+    </row>
+    <row r="6" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1.2</v>
+      </c>
+      <c r="E7" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="33">
+        <v>1.2</v>
+      </c>
+      <c r="G7" s="33">
+        <v>1.4</v>
+      </c>
+      <c r="H7" s="33">
+        <v>1.4</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="20">
-        <v>2019</v>
-      </c>
-      <c r="E4" s="20">
-        <v>2020</v>
-      </c>
-      <c r="F4" s="27">
-        <v>2021</v>
-      </c>
-      <c r="G4" s="20">
-        <v>2022</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="C8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="28">
-        <v>0.7</v>
+      <c r="D8" s="36">
+        <v>0.1</v>
       </c>
-      <c r="E5" s="28">
-        <v>1.2</v>
-      </c>
-      <c r="F5" s="28">
-        <v>0.9</v>
-      </c>
-      <c r="G5" s="29">
-        <v>1</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="28">
-        <v>1.2</v>
-      </c>
-      <c r="E7" s="28">
+      <c r="E8" s="36">
         <v>1.3</v>
       </c>
-      <c r="F7" s="28">
-        <v>1.1000000000000001</v>
+      <c r="F8" s="36">
+        <v>2.2000000000000002</v>
       </c>
-      <c r="G7" s="28">
-        <v>1.2</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="30">
-        <v>0.1</v>
-      </c>
-      <c r="E8" s="30">
-        <v>1.2</v>
-      </c>
-      <c r="F8" s="30">
+      <c r="G8" s="36">
         <v>0.8</v>
       </c>
-      <c r="G8" s="30">
-        <v>0.8</v>
+      <c r="H8" s="36">
+        <v>1.3</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>